<commit_message>
teamCount, maxMember, minMember 동적으로 수정
</commit_message>
<xml_diff>
--- a/로우데이터.xlsx
+++ b/로우데이터.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\BasementChord_TeamMaking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2BD325-58DE-4760-B951-823823FF8E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523E9AAB-0957-4DE5-B8EC-AF73AC03271F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F5C9F2D4-B82B-471C-A404-0C59BE861689}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F5C9F2D4-B82B-471C-A404-0C59BE861689}"/>
   </bookViews>
   <sheets>
     <sheet name="네이밍" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="28">
   <si>
     <t>위영웅</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,12 +145,20 @@
     <t>장정아</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>전이강</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이재홍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +173,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,7 +224,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -223,11 +237,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -245,6 +262,216 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -658,10 +885,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442311EE-82A0-47DC-AB15-3CDAC32D1A8F}">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A26"/>
+      <selection sqref="A1:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -794,6 +1021,16 @@
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -804,220 +1041,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49A00BB-3021-4573-9374-5FC9286E198C}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>6</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B23" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>3</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="B27" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
+      <c r="B28" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1028,11 +1281,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63FF8E14-66BA-4F56-A787-609D0CAA4D7E}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BQ16" sqref="BQ16"/>
+      <selection pane="bottomLeft" sqref="A1:AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1040,7 +1293,7 @@
     <col min="1" max="1" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -1120,8 +1373,14 @@
       <c r="AA1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1203,8 +1462,14 @@
       <c r="AA2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1286,8 +1551,14 @@
       <c r="AA3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -1369,8 +1640,14 @@
       <c r="AA4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1452,8 +1729,14 @@
       <c r="AA5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1535,8 +1818,14 @@
       <c r="AA6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1618,8 +1907,14 @@
       <c r="AA7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1701,8 +1996,14 @@
       <c r="AA8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1784,8 +2085,14 @@
       <c r="AA9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1867,8 +2174,14 @@
       <c r="AA10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1950,8 +2263,14 @@
       <c r="AA11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -2033,8 +2352,14 @@
       <c r="AA12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2116,8 +2441,14 @@
       <c r="AA13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -2199,8 +2530,14 @@
       <c r="AA14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -2282,8 +2619,14 @@
       <c r="AA15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -2365,8 +2708,14 @@
       <c r="AA16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -2448,8 +2797,14 @@
       <c r="AA17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -2531,8 +2886,14 @@
       <c r="AA18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -2614,8 +2975,14 @@
       <c r="AA19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2697,8 +3064,14 @@
       <c r="AA20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -2780,8 +3153,14 @@
       <c r="AA21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2863,8 +3242,14 @@
       <c r="AA22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2946,8 +3331,14 @@
       <c r="AA23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -3029,8 +3420,14 @@
       <c r="AA24" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -3112,8 +3509,14 @@
       <c r="AA25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -3195,8 +3598,14 @@
       <c r="AA26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -3278,25 +3687,217 @@
       <c r="AA27" s="3">
         <v>2</v>
       </c>
+      <c r="AB27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3">
+        <v>0</v>
+      </c>
+      <c r="X28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>1</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="W29" s="3">
+        <v>0</v>
+      </c>
+      <c r="X29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A16:XFD16">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+  <conditionalFormatting sqref="A16:AA16 AD16:XFD16">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:AA27">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+  <conditionalFormatting sqref="B2:AA27 B28:Z29">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:AC29">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3306,11 +3907,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837C573B-11F8-445D-A57D-50BFAE0D198E}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+    <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BL14" sqref="BL14"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:AC29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3318,7 +3919,7 @@
     <col min="1" max="1" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -3398,8 +3999,14 @@
       <c r="AA1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -3481,8 +4088,14 @@
       <c r="AA2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -3564,8 +4177,14 @@
       <c r="AA3" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -3647,8 +4266,14 @@
       <c r="AA4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3730,8 +4355,14 @@
       <c r="AA5" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3813,8 +4444,14 @@
       <c r="AA6" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3896,8 +4533,14 @@
       <c r="AA7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -3979,8 +4622,14 @@
       <c r="AA8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -4062,8 +4711,14 @@
       <c r="AA9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -4145,8 +4800,14 @@
       <c r="AA10" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -4228,8 +4889,14 @@
       <c r="AA11" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -4311,8 +4978,14 @@
       <c r="AA12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -4394,8 +5067,14 @@
       <c r="AA13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -4477,8 +5156,14 @@
       <c r="AA14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -4560,8 +5245,14 @@
       <c r="AA15" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -4643,8 +5334,14 @@
       <c r="AA16" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -4726,8 +5423,14 @@
       <c r="AA17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -4809,8 +5512,14 @@
       <c r="AA18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
@@ -4892,8 +5601,14 @@
       <c r="AA19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -4975,8 +5690,14 @@
       <c r="AA20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5058,8 +5779,14 @@
       <c r="AA21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -5141,8 +5868,14 @@
       <c r="AA22" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -5224,8 +5957,14 @@
       <c r="AA23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -5307,8 +6046,14 @@
       <c r="AA24" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -5390,8 +6135,14 @@
       <c r="AA25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -5473,8 +6224,14 @@
       <c r="AA26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -5556,24 +6313,213 @@
       <c r="AA27" s="3">
         <v>2</v>
       </c>
+      <c r="AB27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="3">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3">
+        <v>0</v>
+      </c>
+      <c r="X28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="3">
+        <v>0</v>
+      </c>
+      <c r="W29" s="3">
+        <v>0</v>
+      </c>
+      <c r="X29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A16:XFD16">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+  <conditionalFormatting sqref="AD16:XFD16 A1:AC29">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AA27">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:AC29">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5584,10 +6530,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9686B533-8004-4D1F-BC97-B2A421D85F30}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection sqref="A1:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5800,9 +6746,25 @@
         <v>1</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A26">
+  <conditionalFormatting sqref="A1:A28">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>